<commit_message>
regenerate instance to have positive aserage demands during the last periods
</commit_message>
<xml_diff>
--- a/Instances/G0041111_NonStationary.xlsx
+++ b/Instances/G0041111_NonStationary.xlsx
@@ -995,7 +995,7 @@
         <v>40</v>
       </c>
       <c r="G2" t="n">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s"/>
       <c r="I2" t="n">
@@ -1022,7 +1022,7 @@
         <v>70</v>
       </c>
       <c r="G3" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s"/>
       <c r="I3" t="n">
@@ -1049,7 +1049,7 @@
         <v>60</v>
       </c>
       <c r="G4" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="H4" t="s"/>
       <c r="I4" t="n">
@@ -1076,7 +1076,7 @@
         <v>30</v>
       </c>
       <c r="G5" t="n">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="H5" t="s"/>
       <c r="I5" t="n">
@@ -1546,16 +1546,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -1581,16 +1581,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -1616,16 +1616,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -1947,16 +1947,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>7.166424999999998</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>3.071324999999999</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>5.118874999999999</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>10.23775</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -1982,16 +1982,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>8.1997825</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>3.5141925</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>5.856987499999999</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>11.713975</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -2017,16 +2017,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>9.129804249999998</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>3.912773249999999</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>6.521288749999998</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>13.0425775</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>

</xml_diff>